<commit_message>
Python updates. Add DRAM wiki images
</commit_message>
<xml_diff>
--- a/3DSystem/DOC/AreaEstimates.xlsx
+++ b/3DSystem/DOC/AreaEstimates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="380" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-26120" yWindow="-21060" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -694,7 +694,7 @@
   <dimension ref="C2:R55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="Q19">
         <f>H42/P19/1000000</f>
-        <v>0.6409601813711403</v>
+        <v>0.71120956668901869</v>
       </c>
     </row>
     <row r="22" spans="3:18">
@@ -862,7 +862,7 @@
       </c>
       <c r="Q22">
         <f>(H42-H41)/(P19*1000000-H41)</f>
-        <v>0.62075164638722358</v>
+        <v>0.69495501420825845</v>
       </c>
     </row>
     <row r="25" spans="3:18">
@@ -970,14 +970,14 @@
         <v>17</v>
       </c>
       <c r="F30">
-        <v>980000</v>
+        <v>1200000</v>
       </c>
       <c r="G30">
         <v>2</v>
       </c>
       <c r="H30">
         <f>F30*G30</f>
-        <v>1960000</v>
+        <v>2400000</v>
       </c>
       <c r="L30">
         <f>2700*2</f>
@@ -1145,7 +1145,7 @@
       </c>
       <c r="H38" s="2">
         <f>SUM(H26:H37)</f>
-        <v>3350840</v>
+        <v>3790840</v>
       </c>
       <c r="M38" t="s">
         <v>37</v>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="H40" s="2">
         <f>H38+H39</f>
-        <v>3680840</v>
+        <v>4120840</v>
       </c>
     </row>
     <row r="41" spans="5:14">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="H42" s="2">
         <f>H40+H41</f>
-        <v>4014590</v>
+        <v>4454590</v>
       </c>
       <c r="M42" s="2" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
DOC: Add future work. XLS: Add PE
</commit_message>
<xml_diff>
--- a/3DSystem/DOC/AreaEstimates.xlsx
+++ b/3DSystem/DOC/AreaEstimates.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Manager" sheetId="2" r:id="rId1"/>
+    <sheet name="PE" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="64">
   <si>
     <t>logs/dfi/dfi_test_area_netlist.rpt:Total cell area:                 24158.880290</t>
   </si>
@@ -277,8 +279,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -329,7 +337,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -346,6 +354,9 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -362,6 +373,9 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -693,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -853,7 +867,7 @@
       </c>
       <c r="Q19">
         <f>H42/P19/1000000</f>
-        <v>0.73036848995753112</v>
+        <v>0.75766995561516115</v>
       </c>
     </row>
     <row r="22" spans="3:18">
@@ -862,7 +876,7 @@
       </c>
       <c r="Q22">
         <f>(H42-H41)/(P19*1000000-H41)</f>
-        <v>0.71519229634126802</v>
+        <v>0.7440304233808066</v>
       </c>
     </row>
     <row r="25" spans="3:18">
@@ -1009,8 +1023,7 @@
         <v>1</v>
       </c>
       <c r="H31">
-        <f>F31*G31</f>
-        <v>179000</v>
+        <v>350000</v>
       </c>
       <c r="L31">
         <f>L29+L30</f>
@@ -1145,7 +1158,7 @@
       </c>
       <c r="H38" s="2">
         <f>SUM(H26:H37)</f>
-        <v>3910840</v>
+        <v>4081840</v>
       </c>
       <c r="M38" t="s">
         <v>37</v>
@@ -1182,7 +1195,7 @@
       </c>
       <c r="H40" s="2">
         <f>H38+H39</f>
-        <v>4240840</v>
+        <v>4411840</v>
       </c>
     </row>
     <row r="41" spans="5:14">
@@ -1211,7 +1224,7 @@
       </c>
       <c r="H42" s="2">
         <f>H40+H41</f>
-        <v>4574590</v>
+        <v>4745590</v>
       </c>
       <c r="M42" s="2" t="s">
         <v>39</v>
@@ -1393,6 +1406,781 @@
       <c r="K55">
         <f>H54/H53</f>
         <v>1.9249999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:R55"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="2" spans="3:17">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="3:17">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="3:17">
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="3:17">
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="3:17">
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="3:17">
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="3:17">
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="3:17">
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="3:17">
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="3:17">
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="3:17">
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="P12" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="3:17">
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="N13" t="s">
+        <v>47</v>
+      </c>
+      <c r="O13" s="7">
+        <f>Q13</f>
+        <v>1.61245154965971</v>
+      </c>
+      <c r="P13" s="7">
+        <v>1.39</v>
+      </c>
+      <c r="Q13" s="7">
+        <f>SQRT(O19)</f>
+        <v>1.61245154965971</v>
+      </c>
+    </row>
+    <row r="14" spans="3:17">
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="3:17">
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="3:17">
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="3:18">
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" t="s">
+        <v>45</v>
+      </c>
+      <c r="L17">
+        <v>12.5</v>
+      </c>
+      <c r="M17">
+        <v>14</v>
+      </c>
+      <c r="N17">
+        <f>L17*M17</f>
+        <v>175</v>
+      </c>
+      <c r="O17">
+        <f>N17/64</f>
+        <v>2.734375</v>
+      </c>
+    </row>
+    <row r="18" spans="3:18">
+      <c r="O18" t="s">
+        <v>47</v>
+      </c>
+      <c r="P18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="3:18">
+      <c r="K19" t="s">
+        <v>46</v>
+      </c>
+      <c r="L19">
+        <v>1.46</v>
+      </c>
+      <c r="M19">
+        <v>1.65</v>
+      </c>
+      <c r="N19">
+        <f>L19*M19</f>
+        <v>2.4089999999999998</v>
+      </c>
+      <c r="O19">
+        <v>2.6</v>
+      </c>
+      <c r="P19">
+        <f>O19*N19</f>
+        <v>6.2633999999999999</v>
+      </c>
+      <c r="Q19">
+        <f>H42/P19/1000000</f>
+        <v>0.3791471085991634</v>
+      </c>
+    </row>
+    <row r="22" spans="3:18">
+      <c r="P22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q22">
+        <f>(H42-H41)/(P19*1000000-H41)</f>
+        <v>0.36653010026634519</v>
+      </c>
+    </row>
+    <row r="25" spans="3:18">
+      <c r="P25" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q25">
+        <f>0.7*P19*1000000</f>
+        <v>4384379.9999999991</v>
+      </c>
+    </row>
+    <row r="26" spans="3:18">
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26">
+        <v>114000</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <f>F26*G26</f>
+        <v>114000</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="3:18">
+      <c r="E27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27">
+        <v>600000</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <f t="shared" ref="H27:H37" si="0">F27*G27</f>
+        <v>600000</v>
+      </c>
+      <c r="L27" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M27" s="4">
+        <f>1/L27</f>
+        <v>200</v>
+      </c>
+      <c r="N27" s="4">
+        <f>M27^2</f>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="28" spans="3:18">
+      <c r="E28" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28">
+        <v>1270</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="29" spans="3:18">
+      <c r="E29" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29">
+        <v>335000</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <f>F29*G29</f>
+        <v>335000</v>
+      </c>
+      <c r="L29">
+        <f>4100*2</f>
+        <v>8200</v>
+      </c>
+      <c r="M29" t="s">
+        <v>32</v>
+      </c>
+      <c r="N29">
+        <f>2048+2048/32+2048/32*2+2048/32</f>
+        <v>2304</v>
+      </c>
+    </row>
+    <row r="30" spans="3:18">
+      <c r="E30" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30">
+        <v>1260000</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="H30">
+        <f>F30*G30</f>
+        <v>2520000</v>
+      </c>
+      <c r="L30">
+        <f>2700*2</f>
+        <v>5400</v>
+      </c>
+      <c r="M30" t="s">
+        <v>33</v>
+      </c>
+      <c r="N30">
+        <v>40</v>
+      </c>
+      <c r="Q30">
+        <f>1.95*N19</f>
+        <v>4.6975499999999997</v>
+      </c>
+      <c r="R30">
+        <f>Q30*0.7</f>
+        <v>3.2882849999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="3:18">
+      <c r="E31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31">
+        <v>179000</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>350000</v>
+      </c>
+      <c r="L31">
+        <f>L29+L30</f>
+        <v>13600</v>
+      </c>
+      <c r="M31" t="s">
+        <v>34</v>
+      </c>
+      <c r="N31">
+        <f>128+2+16+4+1</f>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="32" spans="3:18">
+      <c r="E32" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32">
+        <v>6900</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="0"/>
+        <v>6900</v>
+      </c>
+      <c r="N32">
+        <f>SUM(N29:N31)</f>
+        <v>2495</v>
+      </c>
+    </row>
+    <row r="33" spans="5:14">
+      <c r="E33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33">
+        <v>54000</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="0"/>
+        <v>54000</v>
+      </c>
+    </row>
+    <row r="34" spans="5:14">
+      <c r="E34" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34">
+        <v>24000</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="0"/>
+        <v>24000</v>
+      </c>
+      <c r="M34" t="s">
+        <v>35</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="5:14">
+      <c r="E35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35">
+        <v>12500</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="0"/>
+        <v>12500</v>
+      </c>
+      <c r="M35" t="s">
+        <v>36</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="5:14">
+      <c r="E36" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36">
+        <v>500</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N36" s="2">
+        <f>SUM(N34:N35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="5:14">
+      <c r="E37" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37">
+        <v>63670</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="0"/>
+        <v>63670</v>
+      </c>
+    </row>
+    <row r="38" spans="5:14">
+      <c r="G38" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H38" s="2">
+        <v>2250000</v>
+      </c>
+      <c r="M38" t="s">
+        <v>37</v>
+      </c>
+      <c r="N38">
+        <f>N32+N36</f>
+        <v>2495</v>
+      </c>
+    </row>
+    <row r="39" spans="5:14">
+      <c r="E39" t="s">
+        <v>26</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <f>F39*G39</f>
+        <v>0</v>
+      </c>
+      <c r="M39" t="s">
+        <v>38</v>
+      </c>
+      <c r="N39" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="5:14">
+      <c r="G40" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H40" s="2">
+        <f>H38+H39</f>
+        <v>2250000</v>
+      </c>
+    </row>
+    <row r="41" spans="5:14">
+      <c r="E41" t="s">
+        <v>27</v>
+      </c>
+      <c r="F41">
+        <f>N42</f>
+        <v>124750</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <f>F41*G41</f>
+        <v>124750</v>
+      </c>
+      <c r="N41">
+        <f>N38+N39*N38</f>
+        <v>4990</v>
+      </c>
+    </row>
+    <row r="42" spans="5:14">
+      <c r="G42" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H42" s="2">
+        <f>H40+H41</f>
+        <v>2374750</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N42" s="2">
+        <f>N41/N27*1000000</f>
+        <v>124750</v>
+      </c>
+    </row>
+    <row r="46" spans="5:14">
+      <c r="G46" t="s">
+        <v>54</v>
+      </c>
+      <c r="K46">
+        <v>65</v>
+      </c>
+      <c r="L46">
+        <v>32</v>
+      </c>
+      <c r="M46">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="5:14">
+      <c r="F47" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G47">
+        <v>28</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J47" t="s">
+        <v>52</v>
+      </c>
+      <c r="K47">
+        <v>2</v>
+      </c>
+      <c r="L47">
+        <v>0.66</v>
+      </c>
+      <c r="M47">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="48" spans="5:14">
+      <c r="J48" t="s">
+        <v>53</v>
+      </c>
+      <c r="K48">
+        <v>2</v>
+      </c>
+      <c r="L48">
+        <v>0.5</v>
+      </c>
+      <c r="M48">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="49" spans="5:13">
+      <c r="E49" t="s">
+        <v>55</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H49" s="7">
+        <f>(L49-M49)/(L46-M46)</f>
+        <v>1.7272727272727269E-2</v>
+      </c>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="K49" s="7">
+        <v>1.33</v>
+      </c>
+      <c r="L49" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="M49" s="7">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="50" spans="5:13">
+      <c r="E50" t="s">
+        <v>61</v>
+      </c>
+      <c r="G50" s="8">
+        <v>65</v>
+      </c>
+      <c r="H50" s="7">
+        <f>VLOOKUP($G$46,$J$46:$M$49,2,FALSE)-H49*G50</f>
+        <v>0.2072727272727275</v>
+      </c>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="K50" s="7">
+        <f>AVERAGE(K47:K49)</f>
+        <v>1.7766666666666666</v>
+      </c>
+      <c r="L50" s="7">
+        <f t="shared" ref="L50:M50" si="1">AVERAGE(L47:L49)</f>
+        <v>0.63666666666666671</v>
+      </c>
+      <c r="M50" s="7">
+        <f t="shared" si="1"/>
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="51" spans="5:13">
+      <c r="E51" t="s">
+        <v>58</v>
+      </c>
+      <c r="G51" s="8">
+        <v>31</v>
+      </c>
+      <c r="H51" s="7">
+        <f>$H$49*G51+$H$50</f>
+        <v>0.7427272727272729</v>
+      </c>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+      <c r="L51" s="7"/>
+      <c r="M51" s="7"/>
+    </row>
+    <row r="52" spans="5:13">
+      <c r="G52" s="8">
+        <v>21</v>
+      </c>
+      <c r="H52" s="7">
+        <f>$H$49*G52+$H$50</f>
+        <v>0.57000000000000017</v>
+      </c>
+      <c r="I52" s="7"/>
+      <c r="J52" s="7"/>
+      <c r="K52" s="7"/>
+      <c r="L52" s="7"/>
+      <c r="M52" s="7"/>
+    </row>
+    <row r="53" spans="5:13">
+      <c r="G53" s="8">
+        <v>28</v>
+      </c>
+      <c r="H53" s="7">
+        <f>$H$49*G53+$H$50</f>
+        <v>0.69090909090909103</v>
+      </c>
+    </row>
+    <row r="54" spans="5:13">
+      <c r="G54" s="8">
+        <v>65</v>
+      </c>
+      <c r="H54" s="7">
+        <f>$H$49*G54+$H$50</f>
+        <v>1.33</v>
+      </c>
+      <c r="I54" t="s">
+        <v>62</v>
+      </c>
+      <c r="J54" t="s">
+        <v>63</v>
+      </c>
+      <c r="K54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="5:13">
+      <c r="I55">
+        <v>65</v>
+      </c>
+      <c r="J55">
+        <v>28</v>
+      </c>
+      <c r="K55">
+        <f>H54/H53</f>
+        <v>1.9249999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E4:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="4" spans="5:8">
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="5:8">
+      <c r="E5">
+        <f>Manager!H40</f>
+        <v>4411840</v>
+      </c>
+      <c r="F5">
+        <f>PE!H40</f>
+        <v>2250000</v>
+      </c>
+      <c r="G5">
+        <f>SUM(E5:F5)</f>
+        <v>6661840</v>
+      </c>
+      <c r="H5">
+        <f>G5*H$4</f>
+        <v>6661840</v>
+      </c>
+    </row>
+    <row r="6" spans="5:8">
+      <c r="E6">
+        <f>E5/Manager!O19</f>
+        <v>1696861.5384615385</v>
+      </c>
+      <c r="F6">
+        <f>F5/PE!O19</f>
+        <v>865384.61538461538</v>
+      </c>
+      <c r="G6">
+        <f>SUM(E6:F6)</f>
+        <v>2562246.153846154</v>
+      </c>
+      <c r="H6">
+        <f>G6*H$4</f>
+        <v>2562246.153846154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TEX: Diss - WIP
</commit_message>
<xml_diff>
--- a/3DSystem/DOC/AreaEstimates.xlsx
+++ b/3DSystem/DOC/AreaEstimates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Manager" sheetId="2" r:id="rId1"/>
@@ -255,6 +255,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -766,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:R55"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1545,7 +1546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
@@ -1768,7 +1769,7 @@
         <v>1</v>
       </c>
       <c r="H27">
-        <f t="shared" ref="H27:H37" si="0">F27*G27</f>
+        <f t="shared" ref="H27:H28" si="0">F27*G27</f>
         <v>105000</v>
       </c>
       <c r="I27" s="9">

</xml_diff>

<commit_message>
TEX: rearrange layout - WIP
</commit_message>
<xml_diff>
--- a/3DSystem/DOC/AreaEstimates.xlsx
+++ b/3DSystem/DOC/AreaEstimates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="57220" yWindow="1860" windowWidth="39520" windowHeight="24680" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Manager" sheetId="2" r:id="rId1"/>
@@ -20,8 +20,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Lee Baker</author>
+  </authors>
+  <commentList>
+    <comment ref="F30" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Lee Baker:With 32x256 memories
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="114">
   <si>
     <t>logs/dfi/dfi_test_area_netlist.rpt:Total cell area:                 24158.880290</t>
   </si>
@@ -240,6 +275,129 @@
   </si>
   <si>
     <t>simd_wrapper</t>
+  </si>
+  <si>
+    <t>memory Controller</t>
+  </si>
+  <si>
+    <t>NoC</t>
+  </si>
+  <si>
+    <t>Read Control</t>
+  </si>
+  <si>
+    <t>Write Control</t>
+  </si>
+  <si>
+    <t>Instructio Proc</t>
+  </si>
+  <si>
+    <t>read data proc</t>
+  </si>
+  <si>
+    <t>System Controller</t>
+  </si>
+  <si>
+    <t>Misc</t>
+  </si>
+  <si>
+    <t>TSV</t>
+  </si>
+  <si>
+    <t>Operation Decode</t>
+  </si>
+  <si>
+    <t>return Data Control</t>
+  </si>
+  <si>
+    <t>SIMD Control</t>
+  </si>
+  <si>
+    <t>SIMD</t>
+  </si>
+  <si>
+    <t>Streaming Ops</t>
+  </si>
+  <si>
+    <t>StOp Control</t>
+  </si>
+  <si>
+    <t>LM</t>
+  </si>
+  <si>
+    <t>Memory Area</t>
+  </si>
+  <si>
+    <t>Logic Area</t>
+  </si>
+  <si>
+    <t>Comb</t>
+  </si>
+  <si>
+    <t>Buf/Inv</t>
+  </si>
+  <si>
+    <t>NonComb</t>
+  </si>
+  <si>
+    <t>macro/Blackbox</t>
+  </si>
+  <si>
+    <t>from logs.65nm/manager</t>
+  </si>
+  <si>
+    <t>Memory</t>
+  </si>
+  <si>
+    <t>Logic</t>
+  </si>
+  <si>
+    <t>65nm</t>
+  </si>
+  <si>
+    <t>Breakdown</t>
+  </si>
+  <si>
+    <t>28nm</t>
+  </si>
+  <si>
+    <t>64x256</t>
+  </si>
+  <si>
+    <t>32x256</t>
+  </si>
+  <si>
+    <t>area saving</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>logic</t>
+  </si>
+  <si>
+    <t>Net Interconnect area:      undefined  (Wire load has zero net area)</t>
+  </si>
+  <si>
+    <t>Memory represents</t>
+  </si>
+  <si>
+    <t>Combinational area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buf/Inv area: </t>
+  </si>
+  <si>
+    <t>Noncombinational area:</t>
+  </si>
+  <si>
+    <t>Macro/Black Box area:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total cell area: </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> undefined  (Wire load has zero net area)</t>
   </si>
 </sst>
 </file>
@@ -249,13 +407,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -292,13 +449,39 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -310,7 +493,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -364,8 +547,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -382,8 +577,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -410,6 +611,12 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -436,6 +643,12 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -764,11 +977,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:R55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:AA68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -843,20 +1056,26 @@
       </c>
       <c r="O13" s="7">
         <f>Q13</f>
-        <v>1.61245154965971</v>
+        <v>1.6431676725154984</v>
       </c>
       <c r="P13" s="7">
         <v>1.39</v>
       </c>
       <c r="Q13" s="7">
         <f>SQRT(O19)</f>
-        <v>1.61245154965971</v>
+        <v>1.6431676725154984</v>
       </c>
     </row>
     <row r="14" spans="3:17">
       <c r="C14" t="s">
         <v>12</v>
       </c>
+      <c r="N14" t="s">
+        <v>96</v>
+      </c>
+      <c r="O14">
+        <v>2.79</v>
+      </c>
     </row>
     <row r="15" spans="3:17">
       <c r="C15" t="s">
@@ -865,6 +1084,12 @@
       <c r="L15" t="s">
         <v>44</v>
       </c>
+      <c r="N15" t="s">
+        <v>97</v>
+      </c>
+      <c r="O15">
+        <v>2.68</v>
+      </c>
     </row>
     <row r="16" spans="3:17">
       <c r="C16" t="s">
@@ -909,26 +1134,48 @@
         <v>46</v>
       </c>
       <c r="L19">
-        <v>1.46</v>
+        <v>1.47</v>
       </c>
       <c r="M19">
-        <v>1.65</v>
+        <v>1.6559999999999999</v>
       </c>
       <c r="N19">
         <f>L19*M19</f>
-        <v>2.4089999999999998</v>
+        <v>2.43432</v>
       </c>
       <c r="O19">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
       <c r="P19">
-        <f>O19*N19</f>
-        <v>6.2633999999999999</v>
+        <f>O14*N19*(W52)+N19*O15*(1-W52)</f>
+        <v>6.661495908618436</v>
       </c>
       <c r="Q19">
         <f>H42/P19/1000000</f>
-        <v>0.75766995561516115</v>
-      </c>
+        <v>0.7282892711415293</v>
+      </c>
+      <c r="R19" s="10">
+        <f>K42/(N19*1000000)</f>
+        <v>0.82691056582452782</v>
+      </c>
+    </row>
+    <row r="20" spans="3:18">
+      <c r="L20">
+        <f>L19*SQRT(AVERAGE(O14,O15))</f>
+        <v>2.4310618050555606</v>
+      </c>
+      <c r="M20">
+        <f>M19*SQRT(AVERAGE(O14,O15))</f>
+        <v>2.7386655436544274</v>
+      </c>
+      <c r="P20">
+        <f>L20*M20</f>
+        <v>6.6578652000000007</v>
+      </c>
+      <c r="R20" s="10"/>
+    </row>
+    <row r="21" spans="3:18">
+      <c r="R21" s="10"/>
     </row>
     <row r="22" spans="3:18">
       <c r="P22" s="1" t="s">
@@ -936,19 +1183,26 @@
       </c>
       <c r="Q22">
         <f>(H42-H41)/(P19*1000000-H41)</f>
-        <v>0.7440304233808066</v>
+        <v>0.71395818751931817</v>
+      </c>
+      <c r="R22" s="10">
+        <f>(K42-K41)/(N19*1000000-K41)</f>
+        <v>0.79940917398513955</v>
       </c>
     </row>
     <row r="25" spans="3:18">
       <c r="I25" t="s">
         <v>71</v>
       </c>
+      <c r="K25" t="s">
+        <v>100</v>
+      </c>
       <c r="P25" t="s">
         <v>31</v>
       </c>
       <c r="Q25">
         <f>0.7*P19*1000000</f>
-        <v>4384379.9999999991</v>
+        <v>4663047.1360329045</v>
       </c>
     </row>
     <row r="26" spans="3:18">
@@ -967,7 +1221,11 @@
       </c>
       <c r="I26" s="9">
         <f>H26/$H$42</f>
-        <v>2.4022302811663038E-2</v>
+        <v>2.3497906625090489E-2</v>
+      </c>
+      <c r="K26" s="13">
+        <f>H26*(1-$Q$60)/$O$15+H26*$Q$60/$O$14</f>
+        <v>41686.651106584563</v>
       </c>
       <c r="L26" s="4" t="s">
         <v>41</v>
@@ -984,18 +1242,22 @@
         <v>29</v>
       </c>
       <c r="F27">
-        <v>600000</v>
+        <v>880000</v>
       </c>
       <c r="G27">
         <v>1</v>
       </c>
       <c r="H27">
         <f t="shared" ref="H27:H37" si="0">F27*G27</f>
-        <v>600000</v>
+        <v>880000</v>
       </c>
       <c r="I27" s="9">
         <f t="shared" ref="I27:I41" si="1">H27/$H$42</f>
-        <v>0.12643317269296336</v>
+        <v>0.1813873493866634</v>
+      </c>
+      <c r="K27" s="13">
+        <f t="shared" ref="K27:K41" si="2">H27*(1-$Q$60)/$O$15+H27*$Q$60/$O$14</f>
+        <v>321791.6927525826</v>
       </c>
       <c r="L27" s="4">
         <v>5.0000000000000001E-3</v>
@@ -1014,18 +1276,22 @@
         <v>30</v>
       </c>
       <c r="F28">
-        <v>1270</v>
+        <v>77000</v>
       </c>
       <c r="G28">
         <v>1</v>
       </c>
       <c r="H28">
         <f t="shared" si="0"/>
-        <v>1270</v>
+        <v>77000</v>
       </c>
       <c r="I28" s="9">
         <f t="shared" si="1"/>
-        <v>2.6761688220010581E-4</v>
+        <v>1.5871393071333048E-2</v>
+      </c>
+      <c r="K28" s="13">
+        <f t="shared" si="2"/>
+        <v>28156.773115850978</v>
       </c>
     </row>
     <row r="29" spans="3:18">
@@ -1044,7 +1310,11 @@
       </c>
       <c r="I29" s="9">
         <f t="shared" si="1"/>
-        <v>7.0591854753571215E-2</v>
+        <v>6.9050865959695729E-2</v>
+      </c>
+      <c r="K29" s="13">
+        <f t="shared" si="2"/>
+        <v>122500.24667285813</v>
       </c>
       <c r="L29">
         <f>4100*2</f>
@@ -1062,19 +1332,24 @@
       <c r="E30" t="s">
         <v>17</v>
       </c>
-      <c r="F30">
-        <v>1260000</v>
+      <c r="F30" s="12">
+        <f>1280000-(Y40)</f>
+        <v>1135088</v>
       </c>
       <c r="G30">
         <v>2</v>
       </c>
       <c r="H30">
         <f>F30*G30</f>
-        <v>2520000</v>
+        <v>2270176</v>
       </c>
       <c r="I30" s="9">
         <f t="shared" si="1"/>
-        <v>0.53101932531044616</v>
+        <v>0.46793319009229317</v>
+      </c>
+      <c r="K30" s="13">
+        <f t="shared" si="2"/>
+        <v>830140.65668896236</v>
       </c>
       <c r="L30">
         <f>2700*2</f>
@@ -1088,11 +1363,11 @@
       </c>
       <c r="Q30">
         <f>1.95*N19</f>
-        <v>4.6975499999999997</v>
+        <v>4.7469239999999999</v>
       </c>
       <c r="R30">
         <f>Q30*0.7</f>
-        <v>3.2882849999999997</v>
+        <v>3.3228467999999998</v>
       </c>
     </row>
     <row r="31" spans="3:18">
@@ -1110,7 +1385,11 @@
       </c>
       <c r="I31" s="9">
         <f t="shared" si="1"/>
-        <v>7.3752684070895289E-2</v>
+        <v>7.2142695778786584E-2</v>
+      </c>
+      <c r="K31" s="13">
+        <f t="shared" si="2"/>
+        <v>127985.33234477717</v>
       </c>
       <c r="L31">
         <f>L29+L30</f>
@@ -1140,14 +1419,18 @@
       </c>
       <c r="I32" s="9">
         <f t="shared" si="1"/>
-        <v>1.4539814859690786E-3</v>
+        <v>1.4222417167817926E-3</v>
+      </c>
+      <c r="K32" s="13">
+        <f t="shared" si="2"/>
+        <v>2523.1394090827498</v>
       </c>
       <c r="N32">
         <f>SUM(N29:N31)</f>
         <v>2495</v>
       </c>
     </row>
-    <row r="33" spans="5:14">
+    <row r="33" spans="5:27">
       <c r="E33" t="s">
         <v>19</v>
       </c>
@@ -1163,10 +1446,20 @@
       </c>
       <c r="I33" s="9">
         <f t="shared" si="1"/>
-        <v>1.1378985542366703E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="5:14">
+        <v>1.1130587348727072E-2</v>
+      </c>
+      <c r="K33" s="13">
+        <f t="shared" si="2"/>
+        <v>19746.308418908477</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>104</v>
+      </c>
+      <c r="R33" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="5:27">
       <c r="E34" t="s">
         <v>20</v>
       </c>
@@ -1182,7 +1475,11 @@
       </c>
       <c r="I34" s="9">
         <f t="shared" si="1"/>
-        <v>5.0573269077185349E-3</v>
+        <v>4.9469277105453659E-3</v>
+      </c>
+      <c r="K34" s="13">
+        <f t="shared" si="2"/>
+        <v>8776.1370750704336</v>
       </c>
       <c r="M34" t="s">
         <v>35</v>
@@ -1191,8 +1488,15 @@
         <f>2048*2</f>
         <v>4096</v>
       </c>
-    </row>
-    <row r="35" spans="5:14">
+      <c r="P34" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q34" s="9">
+        <f>I26+I27</f>
+        <v>0.20488525601175389</v>
+      </c>
+    </row>
+    <row r="35" spans="5:27">
       <c r="E35" t="s">
         <v>21</v>
       </c>
@@ -1208,7 +1512,11 @@
       </c>
       <c r="I35" s="9">
         <f t="shared" si="1"/>
-        <v>2.6340244311034034E-3</v>
+        <v>2.576524849242378E-3</v>
+      </c>
+      <c r="K35" s="13">
+        <f t="shared" si="2"/>
+        <v>4570.9047265991849</v>
       </c>
       <c r="M35" t="s">
         <v>36</v>
@@ -1217,8 +1525,19 @@
         <f>12+5+3+2048/32</f>
         <v>84</v>
       </c>
-    </row>
-    <row r="36" spans="5:14">
+      <c r="P35" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q35" s="9">
+        <f>I29</f>
+        <v>6.9050865959695729E-2</v>
+      </c>
+      <c r="AA35">
+        <f>12.5/8</f>
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="36" spans="5:27">
       <c r="E36" t="s">
         <v>22</v>
       </c>
@@ -1234,7 +1553,11 @@
       </c>
       <c r="I36" s="9">
         <f t="shared" si="1"/>
-        <v>1.0536097724413614E-4</v>
+        <v>1.0306099396969512E-4</v>
+      </c>
+      <c r="K36" s="13">
+        <f t="shared" si="2"/>
+        <v>182.83618906396737</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>40</v>
@@ -1243,8 +1566,19 @@
         <f>SUM(N34:N35)</f>
         <v>4180</v>
       </c>
-    </row>
-    <row r="37" spans="5:14">
+      <c r="P36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q36" s="9">
+        <f>I30</f>
+        <v>0.46793319009229317</v>
+      </c>
+      <c r="AA36">
+        <f>14/8</f>
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="37" spans="5:27">
       <c r="E37" t="s">
         <v>23</v>
       </c>
@@ -1260,21 +1594,44 @@
       </c>
       <c r="I37" s="9">
         <f t="shared" si="1"/>
-        <v>1.3416666842268296E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="5:14">
+        <v>1.3123786972100976E-2</v>
+      </c>
+      <c r="K37" s="13">
+        <f t="shared" si="2"/>
+        <v>23282.360315405604</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q37" s="9">
+        <f>I31</f>
+        <v>7.2142695778786584E-2</v>
+      </c>
+      <c r="X37" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y37">
+        <f>37392</f>
+        <v>37392</v>
+      </c>
+      <c r="AA37">
+        <f>AA35*AA36</f>
+        <v>2.734375</v>
+      </c>
+    </row>
+    <row r="38" spans="5:27">
       <c r="G38" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H38" s="2">
         <f>SUM(H26:H37)</f>
-        <v>4081840</v>
+        <v>4187746</v>
       </c>
       <c r="J38" s="9">
         <f>SUM(I26:I37)+I39+I41</f>
-        <v>1</v>
-      </c>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="K38" s="13"/>
       <c r="M38" t="s">
         <v>37</v>
       </c>
@@ -1282,8 +1639,25 @@
         <f>N32+N36</f>
         <v>6675</v>
       </c>
-    </row>
-    <row r="39" spans="5:14">
+      <c r="P38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q38" s="9">
+        <f>I35+I36+I37+I32</f>
+        <v>1.7225614532094841E-2</v>
+      </c>
+      <c r="X38" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y38">
+        <v>28335</v>
+      </c>
+      <c r="AA38">
+        <f>AA37*1000000</f>
+        <v>2734375</v>
+      </c>
+    </row>
+    <row r="39" spans="5:27">
       <c r="E39" t="s">
         <v>26</v>
       </c>
@@ -1299,7 +1673,11 @@
       </c>
       <c r="I39" s="9">
         <f t="shared" si="1"/>
-        <v>6.9538244981129843E-2</v>
+        <v>6.8020256019998782E-2</v>
+      </c>
+      <c r="K39" s="13">
+        <f t="shared" si="2"/>
+        <v>120671.88478221846</v>
       </c>
       <c r="M39" t="s">
         <v>38</v>
@@ -1307,17 +1685,39 @@
       <c r="N39" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="5:14">
+      <c r="P39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q39" s="9">
+        <f>I33+I34</f>
+        <v>1.6077515059272438E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="5:27">
       <c r="G40" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H40" s="2">
         <f>H38+H39</f>
-        <v>4411840</v>
-      </c>
-    </row>
-    <row r="41" spans="5:14">
+        <v>4517746</v>
+      </c>
+      <c r="K40" s="13"/>
+      <c r="P40" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q40" s="9">
+        <f>I28</f>
+        <v>1.5871393071333048E-2</v>
+      </c>
+      <c r="X40" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y40">
+        <f>(Y37-Y38)*16</f>
+        <v>144912</v>
+      </c>
+    </row>
+    <row r="41" spans="5:27">
       <c r="E41" t="s">
         <v>27</v>
       </c>
@@ -1334,20 +1734,35 @@
       </c>
       <c r="I41" s="9">
         <f t="shared" si="1"/>
-        <v>7.0328452310460865E-2</v>
+        <v>6.8793213474771492E-2</v>
+      </c>
+      <c r="K41" s="13">
+        <f>H41</f>
+        <v>333750</v>
       </c>
       <c r="N41">
         <f>N38+N39*N38</f>
         <v>13350</v>
       </c>
-    </row>
-    <row r="42" spans="5:14">
+      <c r="P41" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q41" s="9">
+        <f>I41</f>
+        <v>6.8793213474771492E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="5:27">
       <c r="G42" s="3" t="s">
         <v>37</v>
       </c>
       <c r="H42" s="2">
         <f>H40+H41</f>
-        <v>4745590</v>
+        <v>4851496</v>
+      </c>
+      <c r="K42" s="13">
+        <f>SUM(K26:L41)</f>
+        <v>2012964.9285979646</v>
       </c>
       <c r="M42" s="2" t="s">
         <v>39</v>
@@ -1356,8 +1771,21 @@
         <f>N41/N27*1000000</f>
         <v>333750</v>
       </c>
-    </row>
-    <row r="46" spans="5:14">
+      <c r="P42" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q42" s="9">
+        <f>I39</f>
+        <v>6.8020256019998782E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="5:27">
+      <c r="Q43" s="9">
+        <f>SUM(Q34:Q42)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="5:27">
       <c r="G46" t="s">
         <v>54</v>
       </c>
@@ -1371,7 +1799,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="5:14">
+    <row r="47" spans="5:27">
       <c r="F47" s="1" t="s">
         <v>57</v>
       </c>
@@ -1394,7 +1822,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="48" spans="5:14">
+    <row r="48" spans="5:27">
       <c r="J48" t="s">
         <v>53</v>
       </c>
@@ -1408,7 +1836,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="49" spans="5:13">
+    <row r="49" spans="5:24">
       <c r="E49" t="s">
         <v>55</v>
       </c>
@@ -1433,7 +1861,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="50" spans="5:13">
+    <row r="50" spans="5:24">
       <c r="E50" t="s">
         <v>61</v>
       </c>
@@ -1453,15 +1881,15 @@
         <v>1.7766666666666666</v>
       </c>
       <c r="L50" s="7">
-        <f t="shared" ref="L50:M50" si="2">AVERAGE(L47:L49)</f>
+        <f>AVERAGE(L47:L49)</f>
         <v>0.63666666666666671</v>
       </c>
       <c r="M50" s="7">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(M47:M49)</f>
         <v>0.34</v>
       </c>
     </row>
-    <row r="51" spans="5:13">
+    <row r="51" spans="5:24">
       <c r="E51" t="s">
         <v>58</v>
       </c>
@@ -1477,8 +1905,11 @@
       <c r="K51" s="7"/>
       <c r="L51" s="7"/>
       <c r="M51" s="7"/>
-    </row>
-    <row r="52" spans="5:13">
+      <c r="W51" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="5:24">
       <c r="G52" s="8">
         <v>21</v>
       </c>
@@ -1491,8 +1922,15 @@
       <c r="K52" s="7"/>
       <c r="L52" s="7"/>
       <c r="M52" s="7"/>
-    </row>
-    <row r="53" spans="5:13">
+      <c r="P52" t="s">
+        <v>95</v>
+      </c>
+      <c r="W52" s="15">
+        <f>X59/X62</f>
+        <v>0.51355879341490751</v>
+      </c>
+    </row>
+    <row r="53" spans="5:24">
       <c r="G53" s="8">
         <v>28</v>
       </c>
@@ -1500,8 +1938,14 @@
         <f>$H$49*G53+$H$50</f>
         <v>0.69090909090909103</v>
       </c>
-    </row>
-    <row r="54" spans="5:13">
+      <c r="P53" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q53">
+        <v>1194054.8500000001</v>
+      </c>
+    </row>
+    <row r="54" spans="5:24">
       <c r="G54" s="8">
         <v>65</v>
       </c>
@@ -1518,8 +1962,14 @@
       <c r="K54" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="55" spans="5:13">
+      <c r="P54" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q54">
+        <v>57651.839999999997</v>
+      </c>
+    </row>
+    <row r="55" spans="5:24">
       <c r="I55">
         <v>65</v>
       </c>
@@ -1530,10 +1980,160 @@
         <f>H54/H53</f>
         <v>1.9249999999999998</v>
       </c>
+      <c r="P55" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q55">
+        <v>1050958.46</v>
+      </c>
+    </row>
+    <row r="56" spans="5:24">
+      <c r="P56" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q56">
+        <v>2370165.83</v>
+      </c>
+      <c r="W56" t="s">
+        <v>108</v>
+      </c>
+      <c r="X56">
+        <v>1194054.8478250001</v>
+      </c>
+    </row>
+    <row r="57" spans="5:24">
+      <c r="W57" t="s">
+        <v>109</v>
+      </c>
+      <c r="X57">
+        <v>57651.841992000001</v>
+      </c>
+    </row>
+    <row r="58" spans="5:24">
+      <c r="P58" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q58">
+        <f>SUM(Q53:Q56)</f>
+        <v>4672830.9800000004</v>
+      </c>
+      <c r="W58" t="s">
+        <v>110</v>
+      </c>
+      <c r="X58">
+        <v>1050958.459363</v>
+      </c>
+    </row>
+    <row r="59" spans="5:24">
+      <c r="W59" t="s">
+        <v>111</v>
+      </c>
+      <c r="X59">
+        <v>2370165.828125</v>
+      </c>
+    </row>
+    <row r="60" spans="5:24">
+      <c r="H60" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q60" s="10">
+        <f>Q56/Q58</f>
+        <v>0.50722267510732855</v>
+      </c>
+      <c r="W60" t="s">
+        <v>106</v>
+      </c>
+      <c r="X60" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="61" spans="5:24">
+      <c r="H61" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="62" spans="5:24">
+      <c r="P62" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q62" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="R62" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="W62" t="s">
+        <v>112</v>
+      </c>
+      <c r="X62">
+        <v>4615179.1353129996</v>
+      </c>
+    </row>
+    <row r="63" spans="5:24">
+      <c r="P63" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q63" s="4">
+        <f>H41</f>
+        <v>333750</v>
+      </c>
+      <c r="R63" s="4">
+        <f>Q63</f>
+        <v>333750</v>
+      </c>
+    </row>
+    <row r="64" spans="5:24">
+      <c r="P64" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q64" s="4">
+        <f>(SUM(H26:H37)+H39)*(1-Q60)</f>
+        <v>2226242.7884245669</v>
+      </c>
+      <c r="R64" s="4">
+        <f>Q64/O15</f>
+        <v>830687.60762110702</v>
+      </c>
+    </row>
+    <row r="65" spans="16:18">
+      <c r="P65" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q65" s="4">
+        <f>(SUM(H26:H37)+H39)*(Q60)</f>
+        <v>2291503.2115754331</v>
+      </c>
+      <c r="R65" s="4">
+        <f>Q65/O14</f>
+        <v>821327.31597685779</v>
+      </c>
+    </row>
+    <row r="66" spans="16:18">
+      <c r="Q66" s="4">
+        <f>SUM(Q63:Q65)</f>
+        <v>4851496</v>
+      </c>
+      <c r="R66" s="4">
+        <f>SUM(R63:R65)</f>
+        <v>1985764.9235979649</v>
+      </c>
+    </row>
+    <row r="68" spans="16:18">
+      <c r="Q68" t="s">
+        <v>49</v>
+      </c>
+      <c r="R68" s="10">
+        <f>R66/(N19*1000000)</f>
+        <v>0.81573701222434392</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1544,13 +2144,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:R55"/>
+  <dimension ref="C2:R67"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="5" max="5" width="35" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="3:17">
       <c r="C2" t="s">
@@ -1741,7 +2344,7 @@
         <v>1</v>
       </c>
       <c r="H26">
-        <f>F26*G26</f>
+        <f t="shared" ref="H26:H33" si="0">F26*G26</f>
         <v>550000</v>
       </c>
       <c r="I26" s="9">
@@ -1769,7 +2372,7 @@
         <v>1</v>
       </c>
       <c r="H27">
-        <f t="shared" ref="H27:H28" si="0">F27*G27</f>
+        <f t="shared" si="0"/>
         <v>105000</v>
       </c>
       <c r="I27" s="9">
@@ -1818,7 +2421,7 @@
         <v>1</v>
       </c>
       <c r="H29">
-        <f>F29*G29</f>
+        <f t="shared" si="0"/>
         <v>600000</v>
       </c>
       <c r="I29" s="9">
@@ -1848,7 +2451,7 @@
         <v>32</v>
       </c>
       <c r="H30">
-        <f>F30*G30</f>
+        <f t="shared" si="0"/>
         <v>1344000</v>
       </c>
       <c r="I30" s="9">
@@ -1885,7 +2488,7 @@
         <v>1</v>
       </c>
       <c r="H31">
-        <f>F31*G31</f>
+        <f t="shared" si="0"/>
         <v>17000</v>
       </c>
       <c r="I31" s="9">
@@ -1915,7 +2518,7 @@
         <v>1</v>
       </c>
       <c r="H32">
-        <f>F32*G32</f>
+        <f t="shared" si="0"/>
         <v>64000</v>
       </c>
       <c r="I32" s="9">
@@ -1938,7 +2541,7 @@
         <v>1</v>
       </c>
       <c r="H33">
-        <f>F33*G33</f>
+        <f t="shared" si="0"/>
         <v>251000</v>
       </c>
       <c r="I33" s="9">
@@ -2165,11 +2768,11 @@
         <v>1.7766666666666666</v>
       </c>
       <c r="L50" s="7">
-        <f t="shared" ref="L50:M50" si="2">AVERAGE(L47:L49)</f>
+        <f>AVERAGE(L47:L49)</f>
         <v>0.63666666666666671</v>
       </c>
       <c r="M50" s="7">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(M47:M49)</f>
         <v>0.34</v>
       </c>
     </row>
@@ -2241,6 +2844,93 @@
       <c r="K55">
         <f>H54/H53</f>
         <v>1.9249999999999998</v>
+      </c>
+    </row>
+    <row r="58" spans="5:13">
+      <c r="E58" t="s">
+        <v>82</v>
+      </c>
+      <c r="F58" s="9">
+        <f>I27</f>
+        <v>3.3840947546531303E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="5:13">
+      <c r="E59" t="s">
+        <v>83</v>
+      </c>
+      <c r="F59" s="9">
+        <f>I31+I28</f>
+        <v>1.5792442188381273E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="5:13">
+      <c r="E60" t="s">
+        <v>84</v>
+      </c>
+      <c r="F60" s="9">
+        <f>I33</f>
+        <v>8.0895979373136737E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="5:13">
+      <c r="E61" t="s">
+        <v>85</v>
+      </c>
+      <c r="F61" s="9">
+        <f>I29</f>
+        <v>0.19337684312303602</v>
+      </c>
+    </row>
+    <row r="62" spans="5:13">
+      <c r="E62" t="s">
+        <v>86</v>
+      </c>
+      <c r="F62" s="9">
+        <f>I30</f>
+        <v>0.43316412859560066</v>
+      </c>
+    </row>
+    <row r="63" spans="5:13">
+      <c r="E63" t="s">
+        <v>87</v>
+      </c>
+      <c r="F63" s="9">
+        <f>I32</f>
+        <v>2.0626863266457175E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="5:13">
+      <c r="E64" t="s">
+        <v>88</v>
+      </c>
+      <c r="F64" s="9">
+        <f>I26</f>
+        <v>0.17726210619611635</v>
+      </c>
+    </row>
+    <row r="65" spans="5:6">
+      <c r="E65" t="s">
+        <v>81</v>
+      </c>
+      <c r="F65" s="9">
+        <f>I41</f>
+        <v>4.020626863266457E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="5:6">
+      <c r="E66" t="s">
+        <v>80</v>
+      </c>
+      <c r="F66" s="9">
+        <f>I39</f>
+        <v>4.8344210780759001E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="5:6">
+      <c r="F67" s="9">
+        <f>SUM(F58:F66)</f>
+        <v>0.99999999999999978</v>
       </c>
     </row>
   </sheetData>
@@ -2272,7 +2962,7 @@
     <row r="5" spans="5:8">
       <c r="E5">
         <f>Manager!H40</f>
-        <v>4411840</v>
+        <v>4517746</v>
       </c>
       <c r="F5">
         <f>PE!H40</f>
@@ -2280,17 +2970,17 @@
       </c>
       <c r="G5">
         <f>SUM(E5:F5)</f>
-        <v>7389840</v>
+        <v>7495746</v>
       </c>
       <c r="H5">
         <f>G5*H$4</f>
-        <v>7389840</v>
+        <v>7495746</v>
       </c>
     </row>
     <row r="6" spans="5:8">
       <c r="E6">
         <f>E5/Manager!O19</f>
-        <v>1696861.5384615385</v>
+        <v>1673239.2592592591</v>
       </c>
       <c r="F6">
         <f>F5/PE!O19</f>
@@ -2298,11 +2988,11 @@
       </c>
       <c r="G6">
         <f>SUM(E6:F6)</f>
-        <v>2842246.153846154</v>
+        <v>2818623.8746438744</v>
       </c>
       <c r="H6">
         <f>G6*H$4</f>
-        <v>2842246.153846154</v>
+        <v>2818623.8746438744</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TEX: ETD fixes from Josh
</commit_message>
<xml_diff>
--- a/3DSystem/DOC/AreaEstimates.xlsx
+++ b/3DSystem/DOC/AreaEstimates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="57220" yWindow="1860" windowWidth="39520" windowHeight="24680" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="22120" yWindow="10340" windowWidth="25360" windowHeight="15820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Manager" sheetId="2" r:id="rId1"/>
@@ -310,9 +310,6 @@
     <t>return Data Control</t>
   </si>
   <si>
-    <t>SIMD Control</t>
-  </si>
-  <si>
     <t>SIMD</t>
   </si>
   <si>
@@ -398,6 +395,9 @@
   </si>
   <si>
     <t xml:space="preserve"> undefined  (Wire load has zero net area)</t>
+  </si>
+  <si>
+    <t>SIMD Wrapper</t>
   </si>
 </sst>
 </file>
@@ -1071,7 +1071,7 @@
         <v>12</v>
       </c>
       <c r="N14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O14">
         <v>2.79</v>
@@ -1085,7 +1085,7 @@
         <v>44</v>
       </c>
       <c r="N15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="O15">
         <v>2.68</v>
@@ -1195,7 +1195,7 @@
         <v>71</v>
       </c>
       <c r="K25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P25" t="s">
         <v>31</v>
@@ -1256,7 +1256,7 @@
         <v>0.1813873493866634</v>
       </c>
       <c r="K27" s="13">
-        <f t="shared" ref="K27:K41" si="2">H27*(1-$Q$60)/$O$15+H27*$Q$60/$O$14</f>
+        <f t="shared" ref="K27:K39" si="2">H27*(1-$Q$60)/$O$15+H27*$Q$60/$O$14</f>
         <v>321791.6927525826</v>
       </c>
       <c r="L27" s="4">
@@ -1453,10 +1453,10 @@
         <v>19746.308418908477</v>
       </c>
       <c r="Q33" t="s">
+        <v>103</v>
+      </c>
+      <c r="R33" t="s">
         <v>104</v>
-      </c>
-      <c r="R33" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="34" spans="5:27">
@@ -1608,7 +1608,7 @@
         <v>7.2142695778786584E-2</v>
       </c>
       <c r="X37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Y37">
         <f>37392</f>
@@ -1647,7 +1647,7 @@
         <v>1.7225614532094841E-2</v>
       </c>
       <c r="X38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y38">
         <v>28335</v>
@@ -1710,7 +1710,7 @@
         <v>1.5871393071333048E-2</v>
       </c>
       <c r="X40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Y40">
         <f>(Y37-Y38)*16</f>
@@ -1906,7 +1906,7 @@
       <c r="L51" s="7"/>
       <c r="M51" s="7"/>
       <c r="W51" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="5:24">
@@ -1923,7 +1923,7 @@
       <c r="L52" s="7"/>
       <c r="M52" s="7"/>
       <c r="P52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W52" s="15">
         <f>X59/X62</f>
@@ -1939,7 +1939,7 @@
         <v>0.69090909090909103</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q53">
         <v>1194054.8500000001</v>
@@ -1963,7 +1963,7 @@
         <v>58</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q54">
         <v>57651.839999999997</v>
@@ -1981,7 +1981,7 @@
         <v>1.9249999999999998</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q55">
         <v>1050958.46</v>
@@ -1989,13 +1989,13 @@
     </row>
     <row r="56" spans="5:24">
       <c r="P56" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q56">
         <v>2370165.83</v>
       </c>
       <c r="W56" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X56">
         <v>1194054.8478250001</v>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="57" spans="5:24">
       <c r="W57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X57">
         <v>57651.841992000001</v>
@@ -2018,7 +2018,7 @@
         <v>4672830.9800000004</v>
       </c>
       <c r="W58" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X58">
         <v>1050958.459363</v>
@@ -2026,7 +2026,7 @@
     </row>
     <row r="59" spans="5:24">
       <c r="W59" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X59">
         <v>2370165.828125</v>
@@ -2034,39 +2034,39 @@
     </row>
     <row r="60" spans="5:24">
       <c r="H60" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P60" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q60" s="10">
         <f>Q56/Q58</f>
         <v>0.50722267510732855</v>
       </c>
       <c r="W60" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="X60" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="61" spans="5:24">
       <c r="H61" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="62" spans="5:24">
       <c r="P62" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q62" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="R62" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="Q62" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="R62" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="W62" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="X62">
         <v>4615179.1353129996</v>
@@ -2087,7 +2087,7 @@
     </row>
     <row r="64" spans="5:24">
       <c r="P64" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q64" s="4">
         <f>(SUM(H26:H37)+H39)*(1-Q60)</f>
@@ -2100,7 +2100,7 @@
     </row>
     <row r="65" spans="16:18">
       <c r="P65" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q65" s="4">
         <f>(SUM(H26:H37)+H39)*(Q60)</f>
@@ -2146,8 +2146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:R67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView tabSelected="1" topLeftCell="B33" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2309,7 +2309,7 @@
       </c>
       <c r="Q19">
         <f>H42/P19/1000000</f>
-        <v>0.49537790976147145</v>
+        <v>0.51278059839703682</v>
       </c>
     </row>
     <row r="22" spans="3:18">
@@ -2318,7 +2318,7 @@
       </c>
       <c r="Q22">
         <f>(H42-H41)/(P19*1000000-H41)</f>
-        <v>0.48512295048585602</v>
+        <v>0.5028792975654256</v>
       </c>
     </row>
     <row r="25" spans="3:18">
@@ -2349,7 +2349,7 @@
       </c>
       <c r="I26" s="9">
         <f>H26/$H$42</f>
-        <v>0.17726210619611635</v>
+        <v>0.17124620533976803</v>
       </c>
       <c r="L26" s="4" t="s">
         <v>41</v>
@@ -2377,7 +2377,7 @@
       </c>
       <c r="I27" s="9">
         <f t="shared" ref="I27:I33" si="1">H27/$H$42</f>
-        <v>3.3840947546531303E-2</v>
+        <v>3.2692457383046623E-2</v>
       </c>
       <c r="L27" s="4">
         <v>5.0000000000000001E-3</v>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="I28" s="9">
         <f t="shared" si="1"/>
-        <v>1.0313431633228587E-2</v>
+        <v>9.9634155834046854E-3</v>
       </c>
     </row>
     <row r="29" spans="3:18">
@@ -2426,7 +2426,7 @@
       </c>
       <c r="I29" s="9">
         <f t="shared" si="1"/>
-        <v>0.19337684312303602</v>
+        <v>0.18681404218883785</v>
       </c>
       <c r="L29">
         <f>4100*2</f>
@@ -2456,7 +2456,7 @@
       </c>
       <c r="I30" s="9">
         <f t="shared" si="1"/>
-        <v>0.43316412859560066</v>
+        <v>0.41846345450299682</v>
       </c>
       <c r="L30">
         <f>2700*2</f>
@@ -2493,7 +2493,7 @@
       </c>
       <c r="I31" s="9">
         <f t="shared" si="1"/>
-        <v>5.4790105551526871E-3</v>
+        <v>5.2930645286837393E-3</v>
       </c>
       <c r="L31">
         <f>L29+L30</f>
@@ -2523,7 +2523,7 @@
       </c>
       <c r="I32" s="9">
         <f t="shared" si="1"/>
-        <v>2.0626863266457175E-2</v>
+        <v>1.9926831166809371E-2</v>
       </c>
       <c r="N32">
         <f>SUM(N29:N31)</f>
@@ -2535,24 +2535,24 @@
         <v>72</v>
       </c>
       <c r="F33">
-        <v>251000</v>
+        <v>360000</v>
       </c>
       <c r="G33">
         <v>1</v>
       </c>
       <c r="H33">
         <f t="shared" si="0"/>
-        <v>251000</v>
+        <v>360000</v>
       </c>
       <c r="I33" s="9">
         <f t="shared" si="1"/>
-        <v>8.0895979373136737E-2</v>
+        <v>0.11208842531330272</v>
       </c>
     </row>
     <row r="34" spans="5:14">
       <c r="J34" s="9">
         <f>SUM(I26:I37)+I41+I39</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="M34" t="s">
         <v>35</v>
@@ -2584,11 +2584,11 @@
       </c>
       <c r="H38" s="2">
         <f>SUM(H26:H37)</f>
-        <v>2963000</v>
+        <v>3072000</v>
       </c>
       <c r="I38">
         <f>H38-H29</f>
-        <v>2363000</v>
+        <v>2472000</v>
       </c>
       <c r="M38" t="s">
         <v>37</v>
@@ -2614,7 +2614,7 @@
       </c>
       <c r="I39" s="9">
         <f>H39/$H$42</f>
-        <v>4.8344210780759001E-3</v>
+        <v>4.6703510547209462E-3</v>
       </c>
       <c r="M39" t="s">
         <v>38</v>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="H40" s="2">
         <f>H38+H39</f>
-        <v>2978000</v>
+        <v>3087000</v>
       </c>
     </row>
     <row r="41" spans="5:14">
@@ -2649,7 +2649,7 @@
       </c>
       <c r="I41" s="9">
         <f>H41/$H$42</f>
-        <v>4.020626863266457E-2</v>
+        <v>3.8841752938429203E-2</v>
       </c>
       <c r="N41">
         <f>N38+N39*N38</f>
@@ -2662,7 +2662,7 @@
       </c>
       <c r="H42" s="2">
         <f>H40+H41</f>
-        <v>3102750</v>
+        <v>3211750</v>
       </c>
       <c r="M42" s="2" t="s">
         <v>39</v>
@@ -2852,7 +2852,7 @@
       </c>
       <c r="F58" s="9">
         <f>I27</f>
-        <v>3.3840947546531303E-2</v>
+        <v>3.2692457383046623E-2</v>
       </c>
     </row>
     <row r="59" spans="5:13">
@@ -2861,52 +2861,52 @@
       </c>
       <c r="F59" s="9">
         <f>I31+I28</f>
-        <v>1.5792442188381273E-2</v>
+        <v>1.5256480112088425E-2</v>
       </c>
     </row>
     <row r="60" spans="5:13">
       <c r="E60" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="F60" s="9">
         <f>I33</f>
-        <v>8.0895979373136737E-2</v>
+        <v>0.11208842531330272</v>
       </c>
     </row>
     <row r="61" spans="5:13">
       <c r="E61" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F61" s="9">
         <f>I29</f>
-        <v>0.19337684312303602</v>
+        <v>0.18681404218883785</v>
       </c>
     </row>
     <row r="62" spans="5:13">
       <c r="E62" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F62" s="9">
         <f>I30</f>
-        <v>0.43316412859560066</v>
+        <v>0.41846345450299682</v>
       </c>
     </row>
     <row r="63" spans="5:13">
       <c r="E63" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F63" s="9">
         <f>I32</f>
-        <v>2.0626863266457175E-2</v>
+        <v>1.9926831166809371E-2</v>
       </c>
     </row>
     <row r="64" spans="5:13">
       <c r="E64" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F64" s="9">
         <f>I26</f>
-        <v>0.17726210619611635</v>
+        <v>0.17124620533976803</v>
       </c>
     </row>
     <row r="65" spans="5:6">
@@ -2915,7 +2915,7 @@
       </c>
       <c r="F65" s="9">
         <f>I41</f>
-        <v>4.020626863266457E-2</v>
+        <v>3.8841752938429203E-2</v>
       </c>
     </row>
     <row r="66" spans="5:6">
@@ -2924,13 +2924,13 @@
       </c>
       <c r="F66" s="9">
         <f>I39</f>
-        <v>4.8344210780759001E-3</v>
+        <v>4.6703510547209462E-3</v>
       </c>
     </row>
     <row r="67" spans="5:6">
       <c r="F67" s="9">
         <f>SUM(F58:F66)</f>
-        <v>0.99999999999999978</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2966,15 +2966,15 @@
       </c>
       <c r="F5">
         <f>PE!H40</f>
-        <v>2978000</v>
+        <v>3087000</v>
       </c>
       <c r="G5">
         <f>SUM(E5:F5)</f>
-        <v>7495746</v>
+        <v>7604746</v>
       </c>
       <c r="H5">
         <f>G5*H$4</f>
-        <v>7495746</v>
+        <v>7604746</v>
       </c>
     </row>
     <row r="6" spans="5:8">
@@ -2984,15 +2984,15 @@
       </c>
       <c r="F6">
         <f>F5/PE!O19</f>
-        <v>1145384.6153846153</v>
+        <v>1187307.6923076923</v>
       </c>
       <c r="G6">
         <f>SUM(E6:F6)</f>
-        <v>2818623.8746438744</v>
+        <v>2860546.9515669513</v>
       </c>
       <c r="H6">
         <f>G6*H$4</f>
-        <v>2818623.8746438744</v>
+        <v>2860546.9515669513</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TEX:Fix pe sfu table
</commit_message>
<xml_diff>
--- a/3DSystem/DOC/AreaEstimates.xlsx
+++ b/3DSystem/DOC/AreaEstimates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="22120" yWindow="10340" windowWidth="25360" windowHeight="15820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Manager" sheetId="2" r:id="rId1"/>
@@ -493,8 +493,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="65">
+  <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -584,7 +588,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="65">
+  <cellStyles count="69">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -617,6 +621,8 @@
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -649,6 +655,8 @@
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -980,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:AA68"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1152,11 +1160,11 @@
       </c>
       <c r="Q19">
         <f>H42/P19/1000000</f>
-        <v>0.7282892711415293</v>
+        <v>0.72393589460301333</v>
       </c>
       <c r="R19" s="10">
         <f>K42/(N19*1000000)</f>
-        <v>0.82691056582452782</v>
+        <v>0.82255431891955633</v>
       </c>
     </row>
     <row r="20" spans="3:18">
@@ -1183,11 +1191,11 @@
       </c>
       <c r="Q22">
         <f>(H42-H41)/(P19*1000000-H41)</f>
-        <v>0.71395818751931817</v>
+        <v>0.70937519692222395</v>
       </c>
       <c r="R22" s="10">
         <f>(K42-K41)/(N19*1000000-K41)</f>
-        <v>0.79940917398513955</v>
+        <v>0.79436078285049028</v>
       </c>
     </row>
     <row r="25" spans="3:18">
@@ -1216,12 +1224,12 @@
         <v>1</v>
       </c>
       <c r="H26">
-        <f>F26*G26</f>
+        <f t="shared" ref="H26:H29" si="0">F26*G26</f>
         <v>114000</v>
       </c>
       <c r="I26" s="9">
         <f>H26/$H$42</f>
-        <v>2.3497906625090489E-2</v>
+        <v>2.3639210898256838E-2</v>
       </c>
       <c r="K26" s="13">
         <f>H26*(1-$Q$60)/$O$15+H26*$Q$60/$O$14</f>
@@ -1248,12 +1256,12 @@
         <v>1</v>
       </c>
       <c r="H27">
-        <f t="shared" ref="H27:H37" si="0">F27*G27</f>
+        <f t="shared" si="0"/>
         <v>880000</v>
       </c>
       <c r="I27" s="9">
         <f t="shared" ref="I27:I41" si="1">H27/$H$42</f>
-        <v>0.1813873493866634</v>
+        <v>0.18247811921461418</v>
       </c>
       <c r="K27" s="13">
         <f t="shared" ref="K27:K39" si="2">H27*(1-$Q$60)/$O$15+H27*$Q$60/$O$14</f>
@@ -1287,7 +1295,7 @@
       </c>
       <c r="I28" s="9">
         <f t="shared" si="1"/>
-        <v>1.5871393071333048E-2</v>
+        <v>1.5966835431278741E-2</v>
       </c>
       <c r="K28" s="13">
         <f t="shared" si="2"/>
@@ -1305,12 +1313,12 @@
         <v>1</v>
       </c>
       <c r="H29">
-        <f>F29*G29</f>
+        <f t="shared" si="0"/>
         <v>335000</v>
       </c>
       <c r="I29" s="9">
         <f t="shared" si="1"/>
-        <v>6.9050865959695729E-2</v>
+        <v>6.9466102201017899E-2</v>
       </c>
       <c r="K29" s="13">
         <f t="shared" si="2"/>
@@ -1345,7 +1353,7 @@
       </c>
       <c r="I30" s="9">
         <f t="shared" si="1"/>
-        <v>0.46793319009229317</v>
+        <v>0.47074709859790448</v>
       </c>
       <c r="K30" s="13">
         <f t="shared" si="2"/>
@@ -1375,21 +1383,22 @@
         <v>25</v>
       </c>
       <c r="F31">
-        <v>179000</v>
+        <v>321000</v>
       </c>
       <c r="G31">
         <v>1</v>
       </c>
       <c r="H31">
-        <v>350000</v>
+        <f t="shared" ref="H31:H37" si="3">F31*G31</f>
+        <v>321000</v>
       </c>
       <c r="I31" s="9">
         <f t="shared" si="1"/>
-        <v>7.2142695778786584E-2</v>
+        <v>6.6563041213512669E-2</v>
       </c>
       <c r="K31" s="13">
         <f t="shared" si="2"/>
-        <v>127985.33234477717</v>
+        <v>117380.83337906706</v>
       </c>
       <c r="L31">
         <f>L29+L30</f>
@@ -1414,12 +1423,12 @@
         <v>1</v>
       </c>
       <c r="H32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6900</v>
       </c>
       <c r="I32" s="9">
         <f t="shared" si="1"/>
-        <v>1.4222417167817926E-3</v>
+        <v>1.4307943438418612E-3</v>
       </c>
       <c r="K32" s="13">
         <f t="shared" si="2"/>
@@ -1441,12 +1450,12 @@
         <v>1</v>
       </c>
       <c r="H33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>54000</v>
       </c>
       <c r="I33" s="9">
         <f t="shared" si="1"/>
-        <v>1.1130587348727072E-2</v>
+        <v>1.1197520951805869E-2</v>
       </c>
       <c r="K33" s="13">
         <f t="shared" si="2"/>
@@ -1470,12 +1479,12 @@
         <v>1</v>
       </c>
       <c r="H34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>24000</v>
       </c>
       <c r="I34" s="9">
         <f t="shared" si="1"/>
-        <v>4.9469277105453659E-3</v>
+        <v>4.9766759785803867E-3</v>
       </c>
       <c r="K34" s="13">
         <f t="shared" si="2"/>
@@ -1493,7 +1502,7 @@
       </c>
       <c r="Q34" s="9">
         <f>I26+I27</f>
-        <v>0.20488525601175389</v>
+        <v>0.20611733011287103</v>
       </c>
     </row>
     <row r="35" spans="5:27">
@@ -1507,12 +1516,12 @@
         <v>1</v>
       </c>
       <c r="H35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>12500</v>
       </c>
       <c r="I35" s="9">
         <f t="shared" si="1"/>
-        <v>2.576524849242378E-3</v>
+        <v>2.5920187388439515E-3</v>
       </c>
       <c r="K35" s="13">
         <f t="shared" si="2"/>
@@ -1530,7 +1539,7 @@
       </c>
       <c r="Q35" s="9">
         <f>I29</f>
-        <v>6.9050865959695729E-2</v>
+        <v>6.9466102201017899E-2</v>
       </c>
       <c r="AA35">
         <f>12.5/8</f>
@@ -1548,12 +1557,12 @@
         <v>1</v>
       </c>
       <c r="H36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>500</v>
       </c>
       <c r="I36" s="9">
         <f t="shared" si="1"/>
-        <v>1.0306099396969512E-4</v>
+        <v>1.0368074955375805E-4</v>
       </c>
       <c r="K36" s="13">
         <f t="shared" si="2"/>
@@ -1571,7 +1580,7 @@
       </c>
       <c r="Q36" s="9">
         <f>I30</f>
-        <v>0.46793319009229317</v>
+        <v>0.47074709859790448</v>
       </c>
       <c r="AA36">
         <f>14/8</f>
@@ -1589,12 +1598,12 @@
         <v>1</v>
       </c>
       <c r="H37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>63670</v>
       </c>
       <c r="I37" s="9">
         <f t="shared" si="1"/>
-        <v>1.3123786972100976E-2</v>
+        <v>1.3202706648175551E-2</v>
       </c>
       <c r="K37" s="13">
         <f t="shared" si="2"/>
@@ -1605,7 +1614,7 @@
       </c>
       <c r="Q37" s="9">
         <f>I31</f>
-        <v>7.2142695778786584E-2</v>
+        <v>6.6563041213512669E-2</v>
       </c>
       <c r="X37" t="s">
         <v>100</v>
@@ -1625,11 +1634,11 @@
       </c>
       <c r="H38" s="2">
         <f>SUM(H26:H37)</f>
-        <v>4187746</v>
+        <v>4158746</v>
       </c>
       <c r="J38" s="9">
         <f>SUM(I26:I37)+I39+I41</f>
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
       <c r="K38" s="13"/>
       <c r="M38" t="s">
@@ -1644,7 +1653,7 @@
       </c>
       <c r="Q38" s="9">
         <f>I35+I36+I37+I32</f>
-        <v>1.7225614532094841E-2</v>
+        <v>1.732920048041512E-2</v>
       </c>
       <c r="X38" t="s">
         <v>101</v>
@@ -1673,7 +1682,7 @@
       </c>
       <c r="I39" s="9">
         <f t="shared" si="1"/>
-        <v>6.8020256019998782E-2</v>
+        <v>6.8429294705480315E-2</v>
       </c>
       <c r="K39" s="13">
         <f t="shared" si="2"/>
@@ -1690,7 +1699,7 @@
       </c>
       <c r="Q39" s="9">
         <f>I33+I34</f>
-        <v>1.6077515059272438E-2</v>
+        <v>1.6174196930386256E-2</v>
       </c>
     </row>
     <row r="40" spans="5:27">
@@ -1699,7 +1708,7 @@
       </c>
       <c r="H40" s="2">
         <f>H38+H39</f>
-        <v>4517746</v>
+        <v>4488746</v>
       </c>
       <c r="K40" s="13"/>
       <c r="P40" s="1" t="s">
@@ -1707,7 +1716,7 @@
       </c>
       <c r="Q40" s="9">
         <f>I28</f>
-        <v>1.5871393071333048E-2</v>
+        <v>1.5966835431278741E-2</v>
       </c>
       <c r="X40" t="s">
         <v>102</v>
@@ -1734,7 +1743,7 @@
       </c>
       <c r="I41" s="9">
         <f t="shared" si="1"/>
-        <v>6.8793213474771492E-2</v>
+        <v>6.9206900327133503E-2</v>
       </c>
       <c r="K41" s="13">
         <f>H41</f>
@@ -1749,7 +1758,7 @@
       </c>
       <c r="Q41" s="9">
         <f>I41</f>
-        <v>6.8793213474771492E-2</v>
+        <v>6.9206900327133503E-2</v>
       </c>
     </row>
     <row r="42" spans="5:27">
@@ -1758,11 +1767,11 @@
       </c>
       <c r="H42" s="2">
         <f>H40+H41</f>
-        <v>4851496</v>
+        <v>4822496</v>
       </c>
       <c r="K42" s="13">
         <f>SUM(K26:L41)</f>
-        <v>2012964.9285979646</v>
+        <v>2002360.4296322544</v>
       </c>
       <c r="M42" s="2" t="s">
         <v>39</v>
@@ -1776,13 +1785,13 @@
       </c>
       <c r="Q42" s="9">
         <f>I39</f>
-        <v>6.8020256019998782E-2</v>
+        <v>6.8429294705480315E-2</v>
       </c>
     </row>
     <row r="43" spans="5:27">
       <c r="Q43" s="9">
         <f>SUM(Q34:Q42)</f>
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="46" spans="5:27">
@@ -2091,11 +2100,11 @@
       </c>
       <c r="Q64" s="4">
         <f>(SUM(H26:H37)+H39)*(1-Q60)</f>
-        <v>2226242.7884245669</v>
+        <v>2211952.2460026792</v>
       </c>
       <c r="R64" s="4">
         <f>Q64/O15</f>
-        <v>830687.60762110702</v>
+        <v>825355.3156726415</v>
       </c>
     </row>
     <row r="65" spans="16:18">
@@ -2104,21 +2113,21 @@
       </c>
       <c r="Q65" s="4">
         <f>(SUM(H26:H37)+H39)*(Q60)</f>
-        <v>2291503.2115754331</v>
+        <v>2276793.7539973208</v>
       </c>
       <c r="R65" s="4">
         <f>Q65/O14</f>
-        <v>821327.31597685779</v>
+        <v>816055.10895961314</v>
       </c>
     </row>
     <row r="66" spans="16:18">
       <c r="Q66" s="4">
         <f>SUM(Q63:Q65)</f>
-        <v>4851496</v>
+        <v>4822496</v>
       </c>
       <c r="R66" s="4">
         <f>SUM(R63:R65)</f>
-        <v>1985764.9235979649</v>
+        <v>1975160.4246322548</v>
       </c>
     </row>
     <row r="68" spans="16:18">
@@ -2127,7 +2136,7 @@
       </c>
       <c r="R68" s="10">
         <f>R66/(N19*1000000)</f>
-        <v>0.81573701222434392</v>
+        <v>0.81138076531937242</v>
       </c>
     </row>
   </sheetData>
@@ -2146,8 +2155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:R67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B33" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="H27" sqref="H26:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2962,7 +2971,7 @@
     <row r="5" spans="5:8">
       <c r="E5">
         <f>Manager!H40</f>
-        <v>4517746</v>
+        <v>4488746</v>
       </c>
       <c r="F5">
         <f>PE!H40</f>
@@ -2970,17 +2979,17 @@
       </c>
       <c r="G5">
         <f>SUM(E5:F5)</f>
-        <v>7604746</v>
+        <v>7575746</v>
       </c>
       <c r="H5">
         <f>G5*H$4</f>
-        <v>7604746</v>
+        <v>7575746</v>
       </c>
     </row>
     <row r="6" spans="5:8">
       <c r="E6">
         <f>E5/Manager!O19</f>
-        <v>1673239.2592592591</v>
+        <v>1662498.5185185184</v>
       </c>
       <c r="F6">
         <f>F5/PE!O19</f>
@@ -2988,11 +2997,11 @@
       </c>
       <c r="G6">
         <f>SUM(E6:F6)</f>
-        <v>2860546.9515669513</v>
+        <v>2849806.2108262107</v>
       </c>
       <c r="H6">
         <f>G6*H$4</f>
-        <v>2860546.9515669513</v>
+        <v>2849806.2108262107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>